<commit_message>
Improve support for multiple sibling subranges Fixed Excel Template
</commit_message>
<xml_diff>
--- a/tests/Templates/Subranges_Multiple.xlsx
+++ b/tests/Templates/Subranges_Multiple.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\ClosedXML.Report\tests\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\MKU.ClosedXML.Report\tests\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC255AB-E37D-4654-950B-9B6469ABE1DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED337E6-244B-4A5E-900C-4FBF26BDCF17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Customers">'Sheet 1'!$A$4:$F$13</definedName>
-    <definedName name="Customers_Orders">'Sheet 1'!$A$6:$F$7</definedName>
-    <definedName name="Customers_Visitors">'Sheet 1'!$A$10:$F$11</definedName>
+    <definedName name="Customers">'Sheet 1'!$A$4:$I$13</definedName>
+    <definedName name="Customers_Orders">'Sheet 1'!$A$6:$I$7</definedName>
+    <definedName name="Customers_Visitors">'Sheet 1'!$A$10:$I$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Master-detail report</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>&lt;&lt;group&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Ship Date</t>
+  </si>
+  <si>
+    <t>{{item.ShipDate}}</t>
   </si>
 </sst>
 </file>
@@ -264,9 +270,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,7 +779,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -801,14 +807,14 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -818,58 +824,64 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
@@ -878,10 +890,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
@@ -907,12 +919,11 @@
       <c r="I29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>

</xml_diff>